<commit_message>
decide the paths of all features
</commit_message>
<xml_diff>
--- a/doc/expected_revenue.xlsx
+++ b/doc/expected_revenue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14360" yWindow="160" windowWidth="33200" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20600" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>So we would get 47,000 IP/day   500,000pv/day.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>payment to blogs (10% of income)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -93,18 +89,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>sale number</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>amount</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>contracts/month</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>price/month</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -141,11 +129,23 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>What we can get if we paid 47,000 rmb blog?</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>we would pay 100 rmb to blog give us 100IP/day in a month, or 1 rmb/resume.</t>
+    <t>sales amount</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>companies/month</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>What we can get if we paid 47,000 rmb to blog?</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>we would pay 100 rmb to blog which could give us 100IP/day in a month, or 1 rmb/resume.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>So we could get 47,000 IP/day   500,000pv/day.</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -153,13 +153,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="168" formatCode="[$¥-804]#,##0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="[$¥-804]#,##0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -243,10 +239,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -580,7 +576,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A9" zoomScale="150" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -594,26 +590,26 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20">
       <c r="A1" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -628,7 +624,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -643,7 +639,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -658,7 +654,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -673,7 +669,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -691,10 +687,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="10"/>
@@ -716,7 +712,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="9">
         <f>SUM(D3:D10)</f>
@@ -729,22 +725,22 @@
     </row>
     <row r="13" spans="1:4" ht="20">
       <c r="A13" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -759,7 +755,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -774,7 +770,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -789,7 +785,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -804,7 +800,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -819,7 +815,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="5">
         <v>0.1</v>
@@ -835,16 +831,16 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5"/>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="C22" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D22" s="9">
         <f>SUM(D15:D20)</f>
@@ -857,7 +853,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="C24" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="11">
         <f xml:space="preserve"> D11-D22</f>
@@ -866,7 +862,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="C25" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="11">
         <f>D24*12</f>
@@ -875,7 +871,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="C26" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="12">
         <f>D25/6.8</f>
@@ -884,17 +880,17 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -907,7 +903,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
-    <oddHeader>&amp;LEstimating Revenue of Joblet China</oddHeader>
+    <oddHeader>&amp;LRevenue estimating of Joblet China</oddHeader>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
add tax to cost accounting did some changes for db model
</commit_message>
<xml_diff>
--- a/doc/expected_revenue.xlsx
+++ b/doc/expected_revenue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20600" windowHeight="15400" tabRatio="500"/>
+    <workbookView xWindow="4200" yWindow="1700" windowWidth="20600" windowHeight="15400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>OR 47,000 Resumes,   600,000 Resume in one year.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -122,10 +122,6 @@
   </si>
   <si>
     <t>tax</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -153,7 +149,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="[$¥-804]#,##0"/>
   </numFmts>
@@ -576,8 +576,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -687,10 +687,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="10"/>
@@ -830,25 +830,28 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="C22" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D21" s="9">
         <f>SUM(D15:D20)</f>
         <v>102000</v>
       </c>
     </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D22" s="9">
+        <f>(D11-D21)*B22</f>
+        <v>18400</v>
+      </c>
+    </row>
     <row r="23" spans="1:4">
-      <c r="C23" s="7"/>
+      <c r="B23" s="5"/>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4">
@@ -856,8 +859,8 @@
         <v>2</v>
       </c>
       <c r="D24" s="11">
-        <f xml:space="preserve"> D11-D22</f>
-        <v>368000</v>
+        <f xml:space="preserve"> D11-D21-D22</f>
+        <v>349600</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -866,7 +869,7 @@
       </c>
       <c r="D25" s="11">
         <f>D24*12</f>
-        <v>4416000</v>
+        <v>4195200</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -875,22 +878,22 @@
       </c>
       <c r="D26" s="12">
         <f>D25/6.8</f>
-        <v>649411.76470588241</v>
+        <v>616941.17647058819</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4">

</xml_diff>